<commit_message>
pushed new room in timetabling kb rooms and central
</commit_message>
<xml_diff>
--- a/Raw Data/Timetabling KB Rooms_5205_Central.xlsx
+++ b/Raw Data/Timetabling KB Rooms_5205_Central.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikki/Desktop/Topics/taor_project/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F1028A-B7BC-8E43-BF33-B950CCE2AEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C1E6D1-8593-FD49-85AB-5C142A262E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1140" windowWidth="28800" windowHeight="15380" xr2:uid="{E82492CE-E3CB-4DC0-9AC7-BB30FAAC0434}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="156">
   <si>
     <t>CAMPUS</t>
   </si>
@@ -496,6 +496,12 @@
   </si>
   <si>
     <t>3. PRAM 2324 - MolGenProp</t>
+  </si>
+  <si>
+    <t>7-8 Chambers Street</t>
+  </si>
+  <si>
+    <t>7-8CS_1.01</t>
   </si>
 </sst>
 </file>
@@ -619,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -645,6 +651,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,9 +675,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -703,7 +715,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -809,7 +821,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -951,7 +963,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -959,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E83F524-5142-457A-8BD5-C07BCE54D886}">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C69" zoomScale="66" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4731,6 +4743,29 @@
         <v>31</v>
       </c>
     </row>
+    <row r="86" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D86" s="10">
+        <v>23</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G86" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4739,15 +4774,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100347DA14A51159347908FCB644918D075" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f74c0c6907a9c4c0d2bc11040657d8f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2471f7f-c541-44b1-a67d-1fdff98d7327" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c15f0e2457fdefd102a89a6f1db48816" ns2:_="">
     <xsd:import namespace="b2471f7f-c541-44b1-a67d-1fdff98d7327"/>
@@ -4891,15 +4917,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D824CA44-1B67-4901-A6D6-59CDB2CD0164}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59D7F73A-37FF-4C35-9D22-058FD9EF0CE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4915,4 +4942,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D824CA44-1B67-4901-A6D6-59CDB2CD0164}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
pushed new 40GS room data
</commit_message>
<xml_diff>
--- a/Raw Data/Timetabling KB Rooms_5205_Central.xlsx
+++ b/Raw Data/Timetabling KB Rooms_5205_Central.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikki/Desktop/Topics/taor_project/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C1E6D1-8593-FD49-85AB-5C142A262E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B94B76-FF0C-BB4A-9975-25D986C9EAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1140" windowWidth="28800" windowHeight="15380" xr2:uid="{E82492CE-E3CB-4DC0-9AC7-BB30FAAC0434}"/>
+    <workbookView xWindow="6260" yWindow="820" windowWidth="28800" windowHeight="15380" xr2:uid="{E82492CE-E3CB-4DC0-9AC7-BB30FAAC0434}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="160">
   <si>
     <t>CAMPUS</t>
   </si>
@@ -502,6 +502,18 @@
   </si>
   <si>
     <t>7-8CS_1.01</t>
+  </si>
+  <si>
+    <t>40GS_7.01</t>
+  </si>
+  <si>
+    <t>40GS_7.18</t>
+  </si>
+  <si>
+    <t>3. PRAM 2324 - PPLS</t>
+  </si>
+  <si>
+    <t>3. PRAM 2324 - LLC</t>
   </si>
 </sst>
 </file>
@@ -625,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -651,10 +663,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -971,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E83F524-5142-457A-8BD5-C07BCE54D886}">
-  <dimension ref="A1:Q86"/>
+  <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="C74" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3785,44 +3794,33 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D63" s="7">
-        <v>74</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G63" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="C63" s="6"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="5"/>
+      <c r="Q63" s="9"/>
     </row>
     <row r="64" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D64" s="7">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>113</v>
@@ -3845,10 +3843,10 @@
         <v>83</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D65" s="7">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>113</v>
@@ -3865,52 +3863,28 @@
     </row>
     <row r="66" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>122</v>
+        <v>17</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D66" s="7">
-        <v>458</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="G66" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H66" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J66" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K66" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L66" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M66" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N66" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O66" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P66" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q66" s="5" t="s">
-        <v>31</v>
+      <c r="H66" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="32" x14ac:dyDescent="0.2">
@@ -3918,25 +3892,25 @@
         <v>122</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D67" s="7">
-        <v>96</v>
+        <v>458</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F67" s="6" t="s">
-        <v>60</v>
+      <c r="F67" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="G67" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H67" s="5" t="s">
-        <v>23</v>
+      <c r="H67" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="J67" s="5" t="s">
         <v>25</v>
@@ -3971,16 +3945,16 @@
         <v>144</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D68" s="7">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F68" s="8" t="s">
-        <v>21</v>
+      <c r="F68" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="G68" s="8" t="s">
         <v>120</v>
@@ -3993,6 +3967,9 @@
       </c>
       <c r="K68" s="5" t="s">
         <v>26</v>
+      </c>
+      <c r="L68" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="M68" s="5" t="s">
         <v>27</v>
@@ -4018,10 +3995,10 @@
         <v>144</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D69" s="7">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>20</v>
@@ -4065,10 +4042,10 @@
         <v>144</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D70" s="7">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>20</v>
@@ -4112,10 +4089,10 @@
         <v>144</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D71" s="7">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>20</v>
@@ -4159,10 +4136,10 @@
         <v>144</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D72" s="7">
-        <v>194</v>
+        <v>54</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>20</v>
@@ -4173,17 +4150,14 @@
       <c r="G72" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H72" s="6" t="s">
-        <v>38</v>
+      <c r="H72" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="J72" s="5" t="s">
         <v>25</v>
       </c>
       <c r="K72" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="L72" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="M72" s="5" t="s">
         <v>27</v>
@@ -4209,10 +4183,10 @@
         <v>144</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D73" s="7">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>20</v>
@@ -4259,10 +4233,10 @@
         <v>144</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D74" s="7">
-        <v>303</v>
+        <v>193</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>20</v>
@@ -4306,25 +4280,25 @@
         <v>122</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D75" s="7">
-        <v>60</v>
+        <v>303</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F75" s="6" t="s">
-        <v>60</v>
+      <c r="F75" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="G75" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H75" s="5" t="s">
-        <v>23</v>
+      <c r="H75" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="J75" s="5" t="s">
         <v>25</v>
@@ -4359,22 +4333,25 @@
         <v>145</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D76" s="7">
-        <v>250</v>
+        <v>60</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F76" s="8" t="s">
-        <v>21</v>
+      <c r="F76" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="G76" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H76" s="6" t="s">
-        <v>38</v>
+      <c r="H76" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>26</v>
@@ -4406,7 +4383,7 @@
         <v>145</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D77" s="7">
         <v>250</v>
@@ -4445,7 +4422,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>122</v>
       </c>
@@ -4453,10 +4430,10 @@
         <v>145</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D78" s="7">
-        <v>15</v>
+        <v>250</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>20</v>
@@ -4467,8 +4444,29 @@
       <c r="G78" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H78" s="5" t="s">
-        <v>65</v>
+      <c r="H78" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K78" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L78" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M78" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N78" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O78" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P78" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q78" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:17" ht="16" x14ac:dyDescent="0.2">
@@ -4479,10 +4477,10 @@
         <v>145</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D79" s="7">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>20</v>
@@ -4493,8 +4491,8 @@
       <c r="G79" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H79" s="6" t="s">
-        <v>38</v>
+      <c r="H79" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:17" ht="16" x14ac:dyDescent="0.2">
@@ -4505,10 +4503,10 @@
         <v>145</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D80" s="7">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>20</v>
@@ -4517,27 +4515,24 @@
         <v>21</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D81" s="7">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>20</v>
@@ -4546,7 +4541,7 @@
         <v>21</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>23</v>
@@ -4554,143 +4549,106 @@
       <c r="I81" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K81" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M81" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N81" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O81" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P81" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q81" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="D82" s="7">
-        <v>25</v>
-      </c>
-      <c r="E82" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E82" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F82" s="8" t="s">
         <v>21</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K82" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M82" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N82" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O82" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P82" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q82" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="D83" s="7">
-        <v>150</v>
-      </c>
-      <c r="E83" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E83" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F83" s="8" t="s">
         <v>21</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H83" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K83" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L83" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M83" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N83" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O83" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P83" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q83" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I83" s="5"/>
     </row>
     <row r="84" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D84" s="7">
-        <v>36</v>
-      </c>
-      <c r="E84" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E84" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="H84" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="H84" s="5" t="s">
         <v>23</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K84" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M84" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N84" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O84" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P84" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q84" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="32" x14ac:dyDescent="0.2">
@@ -4698,34 +4656,31 @@
         <v>122</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D85" s="7">
-        <v>129</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>113</v>
+        <v>25</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="J85" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="K85" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="L85" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="M85" s="5" t="s">
         <v>27</v>
@@ -4743,26 +4698,149 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D86" s="7">
+        <v>150</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G86" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K86" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L86" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M86" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N86" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O86" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P86" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q86" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D87" s="7">
+        <v>36</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+      <c r="A88" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D88" s="7">
+        <v>129</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G88" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L88" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M88" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O88" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P88" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q88" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B89" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C89" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D86" s="10">
+      <c r="D89" s="7">
         <v>23</v>
       </c>
-      <c r="E86" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G86" s="8" t="s">
+      <c r="E89" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G89" s="8" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added capacities and enrollment numbers
</commit_message>
<xml_diff>
--- a/Raw Data/Timetabling KB Rooms_5205_Central.xlsx
+++ b/Raw Data/Timetabling KB Rooms_5205_Central.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikki/Desktop/Topics/taor_project/Raw Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1941220_ed_ac_uk/Documents/Year 5/SEM2/Topics in Applied OR/taor_project/taor_project/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B94B76-FF0C-BB4A-9975-25D986C9EAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{48B94B76-FF0C-BB4A-9975-25D986C9EAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2D4329C-A48F-4659-A46A-CBE12958C363}"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="820" windowWidth="28800" windowHeight="15380" xr2:uid="{E82492CE-E3CB-4DC0-9AC7-BB30FAAC0434}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E82492CE-E3CB-4DC0-9AC7-BB30FAAC0434}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="160">
   <si>
     <t>CAMPUS</t>
   </si>
@@ -637,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -661,9 +661,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -980,18 +977,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E83F524-5142-457A-8BD5-C07BCE54D886}">
-  <dimension ref="A1:Q89"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C74" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="17" width="25.83203125" customWidth="1"/>
+    <col min="1" max="17" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1095,7 +1092,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1143,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1197,7 +1194,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -1244,7 +1241,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -1291,7 +1288,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1338,7 +1335,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -1383,7 +1380,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1432,7 +1429,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -1479,7 +1476,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
@@ -1528,7 +1525,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -1575,7 +1572,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -1618,7 +1615,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1665,7 +1662,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1714,7 +1711,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1763,7 +1760,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1804,7 +1801,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1851,7 +1848,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1896,7 +1893,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1935,7 +1932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
@@ -1974,7 +1971,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
@@ -2013,7 +2010,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -2058,7 +2055,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>17</v>
       </c>
@@ -2103,7 +2100,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
@@ -2152,7 +2149,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>17</v>
       </c>
@@ -2201,7 +2198,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>17</v>
       </c>
@@ -2248,7 +2245,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>17</v>
       </c>
@@ -2297,7 +2294,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>17</v>
       </c>
@@ -2344,7 +2341,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>17</v>
       </c>
@@ -2393,7 +2390,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>17</v>
       </c>
@@ -2438,7 +2435,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>17</v>
       </c>
@@ -2483,7 +2480,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>17</v>
       </c>
@@ -2530,7 +2527,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>17</v>
       </c>
@@ -2577,7 +2574,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>17</v>
       </c>
@@ -2624,7 +2621,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>17</v>
       </c>
@@ -2667,7 +2664,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>17</v>
       </c>
@@ -2710,7 +2707,7 @@
       </c>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>17</v>
       </c>
@@ -2755,7 +2752,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>17</v>
       </c>
@@ -2800,7 +2797,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>17</v>
       </c>
@@ -2845,7 +2842,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>17</v>
       </c>
@@ -2890,7 +2887,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>17</v>
       </c>
@@ -2931,7 +2928,7 @@
       </c>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>17</v>
       </c>
@@ -2976,7 +2973,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>17</v>
       </c>
@@ -3021,7 +3018,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>17</v>
       </c>
@@ -3066,7 +3063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>17</v>
       </c>
@@ -3111,7 +3108,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>17</v>
       </c>
@@ -3152,7 +3149,7 @@
       </c>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>17</v>
       </c>
@@ -3195,7 +3192,7 @@
       </c>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>17</v>
       </c>
@@ -3244,7 +3241,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>17</v>
       </c>
@@ -3289,7 +3286,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>17</v>
       </c>
@@ -3334,7 +3331,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>17</v>
       </c>
@@ -3379,7 +3376,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>17</v>
       </c>
@@ -3410,7 +3407,7 @@
       <c r="P53" s="5"/>
       <c r="Q53" s="5"/>
     </row>
-    <row r="54" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>17</v>
       </c>
@@ -3457,7 +3454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>17</v>
       </c>
@@ -3504,7 +3501,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>17</v>
       </c>
@@ -3549,7 +3546,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>17</v>
       </c>
@@ -3596,7 +3593,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>17</v>
       </c>
@@ -3643,7 +3640,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>17</v>
       </c>
@@ -3690,7 +3687,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>17</v>
       </c>
@@ -3733,7 +3730,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>17</v>
       </c>
@@ -3765,7 +3762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>17</v>
       </c>
@@ -3794,33 +3791,44 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="5"/>
-      <c r="Q63" s="9"/>
-    </row>
-    <row r="64" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+      <c r="C63" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D63" s="7">
+        <v>74</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="6" t="s">
         <v>83</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D64" s="7">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>113</v>
@@ -3835,7 +3843,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>17</v>
       </c>
@@ -3843,10 +3851,10 @@
         <v>83</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D65" s="7">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>113</v>
@@ -3861,56 +3869,80 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D66" s="7">
-        <v>45</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>113</v>
+        <v>458</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="G66" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H66" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+      <c r="H66" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M66" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N66" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O66" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P66" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q66" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D67" s="7">
-        <v>458</v>
+        <v>96</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F67" s="8" t="s">
-        <v>21</v>
+      <c r="F67" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="G67" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H67" s="6" t="s">
-        <v>38</v>
+      <c r="H67" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="J67" s="5" t="s">
         <v>25</v>
@@ -3937,7 +3969,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>122</v>
       </c>
@@ -3945,16 +3977,16 @@
         <v>144</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D68" s="7">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F68" s="6" t="s">
-        <v>60</v>
+      <c r="F68" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="G68" s="8" t="s">
         <v>120</v>
@@ -3968,9 +4000,6 @@
       <c r="K68" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L68" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="M68" s="5" t="s">
         <v>27</v>
       </c>
@@ -3987,7 +4016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>122</v>
       </c>
@@ -3995,10 +4024,10 @@
         <v>144</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D69" s="7">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>20</v>
@@ -4034,7 +4063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>122</v>
       </c>
@@ -4042,10 +4071,10 @@
         <v>144</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D70" s="7">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>20</v>
@@ -4081,7 +4110,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>122</v>
       </c>
@@ -4089,10 +4118,10 @@
         <v>144</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D71" s="7">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>20</v>
@@ -4128,7 +4157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>122</v>
       </c>
@@ -4136,10 +4165,10 @@
         <v>144</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D72" s="7">
-        <v>54</v>
+        <v>194</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>20</v>
@@ -4150,8 +4179,8 @@
       <c r="G72" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H72" s="5" t="s">
-        <v>23</v>
+      <c r="H72" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="J72" s="5" t="s">
         <v>25</v>
@@ -4159,6 +4188,9 @@
       <c r="K72" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="L72" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="M72" s="5" t="s">
         <v>27</v>
       </c>
@@ -4175,7 +4207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>122</v>
       </c>
@@ -4183,10 +4215,10 @@
         <v>144</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D73" s="7">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>20</v>
@@ -4225,7 +4257,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>122</v>
       </c>
@@ -4233,10 +4265,10 @@
         <v>144</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D74" s="7">
-        <v>193</v>
+        <v>303</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>20</v>
@@ -4275,30 +4307,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D75" s="7">
-        <v>303</v>
+        <v>60</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F75" s="8" t="s">
-        <v>21</v>
+      <c r="F75" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="G75" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H75" s="6" t="s">
-        <v>38</v>
+      <c r="H75" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="J75" s="5" t="s">
         <v>25</v>
@@ -4325,7 +4357,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>122</v>
       </c>
@@ -4333,25 +4365,22 @@
         <v>145</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D76" s="7">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F76" s="6" t="s">
-        <v>60</v>
+      <c r="F76" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="G76" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H76" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>25</v>
+      <c r="H76" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>26</v>
@@ -4375,7 +4404,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>122</v>
       </c>
@@ -4383,7 +4412,7 @@
         <v>145</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D77" s="7">
         <v>250</v>
@@ -4422,7 +4451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>122</v>
       </c>
@@ -4430,10 +4459,10 @@
         <v>145</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D78" s="7">
-        <v>250</v>
+        <v>15</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>20</v>
@@ -4444,32 +4473,11 @@
       <c r="G78" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H78" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K78" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L78" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M78" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N78" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O78" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P78" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q78" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="H78" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>122</v>
       </c>
@@ -4477,10 +4485,10 @@
         <v>145</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D79" s="7">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>20</v>
@@ -4491,11 +4499,11 @@
       <c r="G79" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H79" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="H79" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>122</v>
       </c>
@@ -4503,10 +4511,10 @@
         <v>145</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D80" s="7">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>20</v>
@@ -4515,13 +4523,16 @@
         <v>21</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>122</v>
       </c>
@@ -4529,10 +4540,10 @@
         <v>145</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="D81" s="7">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>20</v>
@@ -4541,16 +4552,14 @@
         <v>21</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I81" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>122</v>
       </c>
@@ -4558,10 +4567,10 @@
         <v>145</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D82" s="7">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>20</v>
@@ -4570,25 +4579,25 @@
         <v>21</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="I82" s="5"/>
     </row>
-    <row r="83" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D83" s="7">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>20</v>
@@ -4597,14 +4606,34 @@
         <v>21</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I83" s="5"/>
-    </row>
-    <row r="84" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+      <c r="I83" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K83" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M83" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N83" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O83" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P83" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q83" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>122</v>
       </c>
@@ -4612,12 +4641,12 @@
         <v>146</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D84" s="7">
-        <v>35</v>
-      </c>
-      <c r="E84" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E84" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F84" s="8" t="s">
@@ -4651,18 +4680,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D85" s="7">
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="E85" s="7" t="s">
         <v>20</v>
@@ -4671,16 +4700,16 @@
         <v>21</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="H85" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>35</v>
+        <v>151</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="K85" s="5" t="s">
         <v>26</v>
+      </c>
+      <c r="L85" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="M85" s="5" t="s">
         <v>27</v>
@@ -4698,149 +4727,102 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D86" s="7">
+        <v>36</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G86" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="E86" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G86" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H86" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K86" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L86" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M86" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N86" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O86" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P86" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q86" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+      <c r="H86" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D87" s="7">
-        <v>36</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>20</v>
+        <v>129</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>60</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="H87" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K87" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L87" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M87" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N87" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O87" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q87" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="D88" s="7">
-        <v>129</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>113</v>
+        <v>23</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K88" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L88" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M88" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N88" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O88" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P88" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q88" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D89" s="7">
-        <v>23</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F89" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G89" s="8" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4852,6 +4834,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100347DA14A51159347908FCB644918D075" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f74c0c6907a9c4c0d2bc11040657d8f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2471f7f-c541-44b1-a67d-1fdff98d7327" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c15f0e2457fdefd102a89a6f1db48816" ns2:_="">
     <xsd:import namespace="b2471f7f-c541-44b1-a67d-1fdff98d7327"/>
@@ -4995,16 +4986,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D824CA44-1B67-4901-A6D6-59CDB2CD0164}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59D7F73A-37FF-4C35-9D22-058FD9EF0CE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5020,12 +5010,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D824CA44-1B67-4901-A6D6-59CDB2CD0164}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>